<commit_message>
TestNG, data from xlsx - testing
</commit_message>
<xml_diff>
--- a/src/test/java/t08_XlsxData/sample_data.xlsx
+++ b/src/test/java/t08_XlsxData/sample_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>username</t>
   </si>
@@ -19,24 +19,12 @@
     <t>password</t>
   </si>
   <si>
-    <t>scenario</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>aaa@email.com</t>
   </si>
   <si>
     <t>aaaaaa</t>
   </si>
   <si>
-    <t>login</t>
-  </si>
-  <si>
-    <t>login function</t>
-  </si>
-  <si>
     <t>bbb@email.com</t>
   </si>
   <si>
@@ -49,7 +37,10 @@
     <t>cccccc</t>
   </si>
   <si>
-    <t>signup</t>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>admin123</t>
   </si>
 </sst>
 </file>
@@ -317,53 +308,37 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>